<commit_message>
Update excel scenarios - adding no-base-change settlements variants
</commit_message>
<xml_diff>
--- a/data_as_provided/Scenario Baseline - Dwelling+Employment projections.xlsx
+++ b/data_as_provided/Scenario Baseline - Dwelling+Employment projections.xlsx
@@ -1,14 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21917"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\soton.ac.uk\ude\PersonalFiles\Users\ajh9\mydocuments\current\01 mistral\01 CaMKOx\Housing scenarios\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_68BEE42D11540FF5A468BF6F4A86DB4113B856D4" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_B1DCF3B2C0A47C444C0188836947389583E95FB2" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17520" windowHeight="10800" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="66">
   <si>
     <t>Target</t>
   </si>
@@ -222,6 +217,12 @@
     <t>Change</t>
   </si>
   <si>
+    <t>2050 people</t>
+  </si>
+  <si>
+    <t>2017 people</t>
+  </si>
+  <si>
     <t>Estimated number of employed people by local authorities in Arc</t>
   </si>
   <si>
@@ -340,7 +341,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -393,6 +394,10 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -9117,11 +9122,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="330822376"/>
-        <c:axId val="330822768"/>
+        <c:axId val="155520000"/>
+        <c:axId val="155534080"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="330822376"/>
+        <c:axId val="155520000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9161,7 +9166,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330822768"/>
+        <c:crossAx val="155534080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9169,7 +9174,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="330822768"/>
+        <c:axId val="155534080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2500000"/>
@@ -9267,7 +9272,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="330822376"/>
+        <c:crossAx val="155520000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -17758,8 +17763,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="496512096"/>
-        <c:axId val="496512488"/>
+        <c:axId val="157830144"/>
+        <c:axId val="157836032"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredAreaSeries>
@@ -18117,7 +18122,7 @@
         </c:extLst>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="496512096"/>
+        <c:axId val="157830144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18157,7 +18162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496512488"/>
+        <c:crossAx val="157836032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18165,7 +18170,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="496512488"/>
+        <c:axId val="157836032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3500000"/>
@@ -18263,7 +18268,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496512096"/>
+        <c:crossAx val="157830144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -19499,7 +19504,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="154" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19510,7 +19515,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="154" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19574,7 +19579,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9311355" cy="6079977"/>
+    <xdr:ext cx="9296153" cy="6073734"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -19607,7 +19612,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9311355" cy="6079977"/>
+    <xdr:ext cx="9296153" cy="6073734"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -25811,17 +25816,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AV61"/>
+  <dimension ref="A1:AV62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A17" sqref="A17"/>
+      <selection pane="topRight" activeCell="I35" sqref="I35:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="25.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="48" width="10.85546875" style="12" customWidth="1"/>
+    <col min="2" max="8" width="10.85546875" style="12" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="12" customWidth="1"/>
+    <col min="11" max="48" width="10.85546875" style="12" customWidth="1"/>
     <col min="49" max="16384" width="8.85546875" style="12"/>
   </cols>
   <sheetData>
@@ -31242,6 +31250,12 @@
       <c r="H35" s="27" t="s">
         <v>60</v>
       </c>
+      <c r="I35" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="J35" s="37" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="36" spans="1:34">
       <c r="A36" s="28" t="s">
@@ -31272,6 +31286,14 @@
         <f>SUM(G36-D36)/D36</f>
         <v>0.29824005073727622</v>
       </c>
+      <c r="I36" s="36">
+        <f>G36*B36</f>
+        <v>191622.82796892343</v>
+      </c>
+      <c r="J36" s="12">
+        <f>D36*B36</f>
+        <v>147602</v>
+      </c>
     </row>
     <row r="37" spans="1:34">
       <c r="A37" s="28" t="s">
@@ -31302,6 +31324,14 @@
         <f t="shared" ref="H37:H61" si="4">SUM(G37-D37)/D37</f>
         <v>0.15410573678290221</v>
       </c>
+      <c r="I37" s="36">
+        <f t="shared" ref="I37:I61" si="5">G37*B37</f>
+        <v>178403.97300337459</v>
+      </c>
+      <c r="J37" s="12">
+        <f t="shared" ref="J37:J61" si="6">D37*B37</f>
+        <v>154582</v>
+      </c>
     </row>
     <row r="38" spans="1:34">
       <c r="A38" s="28" t="s">
@@ -31332,6 +31362,14 @@
         <f t="shared" si="4"/>
         <v>0.25780818709537107</v>
       </c>
+      <c r="I38" s="36">
+        <f t="shared" si="5"/>
+        <v>175800.07688575872</v>
+      </c>
+      <c r="J38" s="12">
+        <f t="shared" si="6"/>
+        <v>139767</v>
+      </c>
     </row>
     <row r="39" spans="1:34">
       <c r="A39" s="28" t="s">
@@ -31362,6 +31400,14 @@
         <f t="shared" si="4"/>
         <v>0.3843854244517762</v>
       </c>
+      <c r="I39" s="36">
+        <f t="shared" si="5"/>
+        <v>181668.74609453324</v>
+      </c>
+      <c r="J39" s="12">
+        <f t="shared" si="6"/>
+        <v>131227</v>
+      </c>
     </row>
     <row r="40" spans="1:34">
       <c r="A40" s="28" t="s">
@@ -31392,6 +31438,14 @@
         <f t="shared" si="4"/>
         <v>0.28439284434985956</v>
       </c>
+      <c r="I40" s="36">
+        <f t="shared" si="5"/>
+        <v>140340.46853073177</v>
+      </c>
+      <c r="J40" s="12">
+        <f t="shared" si="6"/>
+        <v>109266.00000000001</v>
+      </c>
     </row>
     <row r="41" spans="1:34">
       <c r="A41" s="28" t="s">
@@ -31422,6 +31476,14 @@
         <f t="shared" si="4"/>
         <v>0.39910028163988337</v>
       </c>
+      <c r="I41" s="36">
+        <f t="shared" si="5"/>
+        <v>274251.63720704993</v>
+      </c>
+      <c r="J41" s="12">
+        <f t="shared" si="6"/>
+        <v>196020</v>
+      </c>
     </row>
     <row r="42" spans="1:34">
       <c r="A42" s="8" t="s">
@@ -31452,6 +31514,14 @@
         <f t="shared" si="4"/>
         <v>0.22566830144366928</v>
       </c>
+      <c r="I42" s="36">
+        <f t="shared" si="5"/>
+        <v>214195.34102369277</v>
+      </c>
+      <c r="J42" s="12">
+        <f t="shared" si="6"/>
+        <v>174758</v>
+      </c>
     </row>
     <row r="43" spans="1:34">
       <c r="A43" s="8" t="s">
@@ -31482,6 +31552,14 @@
         <f t="shared" si="4"/>
         <v>0.14992766313865835</v>
       </c>
+      <c r="I43" s="36">
+        <f t="shared" si="5"/>
+        <v>109651.35231858677</v>
+      </c>
+      <c r="J43" s="12">
+        <f t="shared" si="6"/>
+        <v>95355</v>
+      </c>
     </row>
     <row r="44" spans="1:34">
       <c r="A44" s="8" t="s">
@@ -31512,6 +31590,14 @@
         <f t="shared" si="4"/>
         <v>0.25797445382843598</v>
       </c>
+      <c r="I44" s="36">
+        <f t="shared" si="5"/>
+        <v>87787.747260417396</v>
+      </c>
+      <c r="J44" s="12">
+        <f t="shared" si="6"/>
+        <v>69785</v>
+      </c>
     </row>
     <row r="45" spans="1:34">
       <c r="A45" s="34" t="s">
@@ -31542,6 +31628,14 @@
         <f t="shared" si="4"/>
         <v>0.36053633504386684</v>
       </c>
+      <c r="I45" s="36">
+        <f t="shared" si="5"/>
+        <v>231171.4497599735</v>
+      </c>
+      <c r="J45" s="12">
+        <f t="shared" si="6"/>
+        <v>169912</v>
+      </c>
     </row>
     <row r="46" spans="1:34">
       <c r="A46" s="34" t="s">
@@ -31572,6 +31666,14 @@
         <f t="shared" si="4"/>
         <v>0.36490656608949062</v>
       </c>
+      <c r="I46" s="36">
+        <f t="shared" si="5"/>
+        <v>382214.78570204007</v>
+      </c>
+      <c r="J46" s="12">
+        <f t="shared" si="6"/>
+        <v>280030</v>
+      </c>
     </row>
     <row r="47" spans="1:34">
       <c r="A47" s="28" t="s">
@@ -31602,6 +31704,14 @@
         <f t="shared" si="4"/>
         <v>0.26899563318777281</v>
       </c>
+      <c r="I47" s="36">
+        <f t="shared" si="5"/>
+        <v>104867.26113537117</v>
+      </c>
+      <c r="J47" s="12">
+        <f t="shared" si="6"/>
+        <v>82638</v>
+      </c>
     </row>
     <row r="48" spans="1:34">
       <c r="A48" s="35" t="s">
@@ -31632,8 +31742,16 @@
         <f t="shared" si="4"/>
         <v>0.16810874462420641</v>
       </c>
+      <c r="I48" s="36">
+        <f t="shared" si="5"/>
+        <v>250743.88690354291</v>
+      </c>
+      <c r="J48" s="12">
+        <f t="shared" si="6"/>
+        <v>214658.00000000003</v>
+      </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:10">
       <c r="A49" s="35" t="s">
         <v>31</v>
       </c>
@@ -31662,8 +31780,16 @@
         <f t="shared" si="4"/>
         <v>0.44754388352156765</v>
       </c>
+      <c r="I49" s="36">
+        <f t="shared" si="5"/>
+        <v>387248.3872635733</v>
+      </c>
+      <c r="J49" s="12">
+        <f t="shared" si="6"/>
+        <v>267521</v>
+      </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:10">
       <c r="A50" s="28" t="s">
         <v>32</v>
       </c>
@@ -31692,8 +31818,16 @@
         <f t="shared" si="4"/>
         <v>0.22465437788018428</v>
       </c>
+      <c r="I50" s="36">
+        <f t="shared" si="5"/>
+        <v>276350.60829493089</v>
+      </c>
+      <c r="J50" s="12">
+        <f t="shared" si="6"/>
+        <v>225656</v>
+      </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:10">
       <c r="A51" s="28" t="s">
         <v>33</v>
       </c>
@@ -31722,8 +31856,16 @@
         <f t="shared" si="4"/>
         <v>0.27666955767562867</v>
       </c>
+      <c r="I51" s="36">
+        <f t="shared" si="5"/>
+        <v>116271.40329575021</v>
+      </c>
+      <c r="J51" s="12">
+        <f t="shared" si="6"/>
+        <v>91074</v>
+      </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:10">
       <c r="A52" s="28" t="s">
         <v>34</v>
       </c>
@@ -31752,8 +31894,16 @@
         <f t="shared" si="4"/>
         <v>0.2327571255130948</v>
       </c>
+      <c r="I52" s="36">
+        <f t="shared" si="5"/>
+        <v>97281.795802740351</v>
+      </c>
+      <c r="J52" s="12">
+        <f t="shared" si="6"/>
+        <v>78914</v>
+      </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:10">
       <c r="A53" s="8" t="s">
         <v>35</v>
       </c>
@@ -31782,8 +31932,16 @@
         <f t="shared" si="4"/>
         <v>0.38386070569950703</v>
       </c>
+      <c r="I53" s="36">
+        <f t="shared" si="5"/>
+        <v>275269.26841351175</v>
+      </c>
+      <c r="J53" s="12">
+        <f t="shared" si="6"/>
+        <v>198914</v>
+      </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:10">
       <c r="A54" s="8" t="s">
         <v>36</v>
       </c>
@@ -31812,8 +31970,16 @@
         <f t="shared" si="4"/>
         <v>0.36239001432371593</v>
       </c>
+      <c r="I54" s="36">
+        <f t="shared" si="5"/>
+        <v>136582.32371598115</v>
+      </c>
+      <c r="J54" s="12">
+        <f t="shared" si="6"/>
+        <v>100252</v>
+      </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:10">
       <c r="A55" s="8" t="s">
         <v>37</v>
       </c>
@@ -31842,8 +32008,16 @@
         <f t="shared" si="4"/>
         <v>0.47792706333973134</v>
       </c>
+      <c r="I55" s="36">
+        <f t="shared" si="5"/>
+        <v>102775.04798464492</v>
+      </c>
+      <c r="J55" s="12">
+        <f t="shared" si="6"/>
+        <v>69540</v>
+      </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:10">
       <c r="A56" s="8" t="s">
         <v>38</v>
       </c>
@@ -31872,8 +32046,16 @@
         <f t="shared" si="4"/>
         <v>0.29443374226908636</v>
       </c>
+      <c r="I56" s="36">
+        <f t="shared" si="5"/>
+        <v>120557.08658623137</v>
+      </c>
+      <c r="J56" s="12">
+        <f t="shared" si="6"/>
+        <v>93135</v>
+      </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:10">
       <c r="A57" s="8" t="s">
         <v>39</v>
       </c>
@@ -31902,8 +32084,16 @@
         <f t="shared" si="4"/>
         <v>0.29178444630379202</v>
       </c>
+      <c r="I57" s="36">
+        <f t="shared" si="5"/>
+        <v>130180.86936071096</v>
+      </c>
+      <c r="J57" s="12">
+        <f t="shared" si="6"/>
+        <v>100776</v>
+      </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:10">
       <c r="A58" s="28" t="s">
         <v>40</v>
       </c>
@@ -31932,8 +32122,16 @@
         <f t="shared" si="4"/>
         <v>0.42225766032577744</v>
       </c>
+      <c r="I58" s="36">
+        <f t="shared" si="5"/>
+        <v>177667.00467023579</v>
+      </c>
+      <c r="J58" s="12">
+        <f t="shared" si="6"/>
+        <v>124919</v>
+      </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:10">
       <c r="A59" s="28" t="s">
         <v>41</v>
       </c>
@@ -31962,8 +32160,16 @@
         <f t="shared" si="4"/>
         <v>0.26760109553729655</v>
       </c>
+      <c r="I59" s="36">
+        <f t="shared" si="5"/>
+        <v>112636.49814725311</v>
+      </c>
+      <c r="J59" s="12">
+        <f t="shared" si="6"/>
+        <v>88858</v>
+      </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:10">
       <c r="A60" s="28" t="s">
         <v>43</v>
       </c>
@@ -31992,8 +32198,16 @@
         <f t="shared" si="4"/>
         <v>0.29575326595022178</v>
       </c>
+      <c r="I60" s="36">
+        <f t="shared" si="5"/>
+        <v>229321.11725460429</v>
+      </c>
+      <c r="J60" s="12">
+        <f t="shared" si="6"/>
+        <v>176979</v>
+      </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:10">
       <c r="A61" s="28" t="s">
         <v>45</v>
       </c>
@@ -32021,6 +32235,24 @@
       <c r="H61" s="33">
         <f t="shared" si="4"/>
         <v>0.36945902484905502</v>
+      </c>
+      <c r="I61" s="36">
+        <f t="shared" si="5"/>
+        <v>214601.07648897116</v>
+      </c>
+      <c r="J61" s="12">
+        <f t="shared" si="6"/>
+        <v>156705</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="I62" s="36">
+        <f>SUM(I36:I61)</f>
+        <v>4899462.0410731351</v>
+      </c>
+      <c r="J62" s="36">
+        <f>SUM(J36:J61)</f>
+        <v>3738843</v>
       </c>
     </row>
   </sheetData>
@@ -32047,12 +32279,12 @@
   <sheetData>
     <row r="1" spans="1:48" ht="12" customHeight="1">
       <c r="A1" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:48" ht="12" customHeight="1">
       <c r="A3" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:48" ht="12" customHeight="1">
@@ -37089,12 +37321,12 @@
   <sheetData>
     <row r="1" spans="1:48">
       <c r="A1" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:48">
       <c r="A3" s="11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:48">

</xml_diff>